<commit_message>
add button to return from movie page
</commit_message>
<xml_diff>
--- a/data/attractions.xlsx
+++ b/data/attractions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesautry/Documents/disney+_picker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721AE0D9-8A70-1A43-B490-4A9022C09471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08609D15-74FB-1C4C-8F24-6EB3354F5198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="800" windowWidth="26180" windowHeight="16960" xr2:uid="{81374443-5BAD-F645-8616-63112015840A}"/>
+    <workbookView xWindow="33280" yWindow="-16860" windowWidth="43800" windowHeight="22940" xr2:uid="{81374443-5BAD-F645-8616-63112015840A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -473,6 +473,45 @@
   </si>
   <si>
     <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/magic-kingdom/cinderella-castle/castle-partners-statue-16x9.jpg?1611845187786</t>
+  </si>
+  <si>
+    <t>Tomorrowland</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/dumbo-the-flying-elephant/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/magic-kingdom/dumbo-the-flying-elephant/dumbo-the-flying-elephant-gallery06.jpg?1550820961335</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/enchanted-tales-with-belle/</t>
+  </si>
+  <si>
+    <t>https://www.tripsavvy.com/thmb/TRwzYMvBr04zEAap2z23uDDPVjM=/2700x1887/filters:fill(auto,1)/Enchanted-Tales-with-Belle-Disney-World-58bdeef73df78c353cdda5cd.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/magic-kingdom/its-a-small-world/its-a-small-world-00.jpg?1634639538944</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/its-a-small-world/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/magic-kingdom/mad-tea-party/mad-tea-party-00.jpg?1634619687993</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/mad-tea-party/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/mickeys-philharmagic/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/magic-kingdom/mickeys-philharmagic/mickeys-philharmagic-gallery01.jpg?1551208516468</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/magic-kingdom/peter-pans-flight/peter-pans-flight-gallery03.jpg?1559892376214</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/magic-kingdom/peter-pan-flight/</t>
   </si>
 </sst>
 </file>
@@ -828,7 +867,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,8 +1192,14 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1167,8 +1212,14 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1181,8 +1232,14 @@
       <c r="D18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1195,8 +1252,14 @@
       <c r="D19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1209,8 +1272,14 @@
       <c r="D20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1223,8 +1292,14 @@
       <c r="D21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1238,7 +1313,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1252,7 +1327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1266,7 +1341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1280,7 +1355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1294,7 +1369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1308,7 +1383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1322,7 +1397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1330,13 +1405,13 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1344,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1358,13 +1433,13 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1372,7 +1447,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
@@ -1386,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>40</v>
@@ -1400,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D34" t="s">
         <v>41</v>
@@ -1414,7 +1489,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
add disney link to attraction
- user can now click on attraction name to see disney website of attraction
- resize movie page for mobile
- documentation on dis_picker
</commit_message>
<xml_diff>
--- a/data/attractions.xlsx
+++ b/data/attractions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesautry/Documents/disney+_picker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C560111-BC30-9E4B-9376-B5288A13B52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF1F358-AE5F-9042-BC04-55599A59F246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35440" windowHeight="16220" xr2:uid="{81374443-5BAD-F645-8616-63112015840A}"/>
+    <workbookView xWindow="36700" yWindow="-14300" windowWidth="43300" windowHeight="20880" xr2:uid="{81374443-5BAD-F645-8616-63112015840A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$86</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="283">
   <si>
     <t>id</t>
   </si>
@@ -313,9 +313,6 @@
     <t>For the First Time in Forever: A Frozen Sing-Along Celebration</t>
   </si>
   <si>
-    <t>Jedi Training: Trials of the Temple</t>
-  </si>
-  <si>
     <t>Grand Avenue</t>
   </si>
   <si>
@@ -716,6 +713,180 @@
   </si>
   <si>
     <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/epcot/frozen-ever-after/frozen-ever-after-olaf-anna-elsa-16x9.jpg?1635179489414</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/reflections-of-china/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/epcot/reflections-of-china/reflections-of-china-gallery01.jpg?1551208546463</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/american-adventure/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/epcot/the-american-adventure/american-adventure-gallery01.jpg?1551208576543</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/impressions-de-france/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/epcot/impressions-de-france/impressions-de-france-gallery01.jpg?1586806691062</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/beauty-and-the-beast-sing-along/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/epcot/beauty-and-the-beast-sing-along/Beauty-and-the-Beast-Sing-Along-16x9.jpg?1632337504571</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/remys-ratatouille-adventure/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/epcot/remys-ratatouille-adventure/RatatouilleKV_16x9.jpg?1643139695472</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/epcot/canada-far-and-wide/canada-far-and-wide-16x9.jpg?1613071634869</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/epcot/canada-far-and-wide/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/vision-dam/digital/parks-platform/parks-global-assets/disney-world/0618ZP_0087DR_JLM_WDW-82237-16x9.jpg?2021-06-30T18:02:29+00:00</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/entertainment/epcot/harmonious/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/its-tough-to-be-a-bug/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/animal-kingdom/its-tough-to-be-a-bug/its-tough-to-be-a-bug-00.jpg?1634619911071</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/discovery-island-trails/</t>
+  </si>
+  <si>
+    <t>https://e6zrk7x26xe.exactdn.com/reports13/animal_kingdom_rivers_light_stadium-57.jpg?strip=all&amp;lossy=1&amp;w=1920&amp;ssl=1</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/animal-kingdom/tree-of-life/tree-of-life-00.jpg?1632755874244</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/tree-of-life/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/animal-kingdom/flight-of-passage/flight-of-passage-in-ride-16x9.jpg?1639083470749</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/avatar-flight-of-passage/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/animal-kingdom/navi-river-journey/pandora-navi-river-journey-full-boat-16x9.jpg?1634752135995</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/navi-river-journey/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/attractions/animal-kingdom/the-boneyard/the-boneyard-00.jpg?1632755812605</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/animal-kingdom/boneyard/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/shops/animal-kingdom/chester-and-hesters-dinosaur-treasures/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/things-to-do/more/shops/animal-kingdom/chester-and-hester-dinosaur-treasures/chester-and-hesters-dinosaur-treasures-00.jpg?1583973826499</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/mickey-minnies-runaway-railway/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/media/blog/wp-content/uploads/2019/12/mbhgyu7898-624x350-624x350.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/media/blog/wp-content/uploads/2017/11/11_17_WDI_9004_1280.jpg</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/star-tours/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/entertainment/hollywood-studios/indiana-jones-epic-stunt-spectacular/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/entertainment/hollywood-studios/indiana-jones-stunt-spectacular-gallery02.jpg?1640811572364</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/entertainment/hollywood-studios/frozen-sing-along-celebration/summer-update-00.jpg?1641315717037</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/entertainment/hollywood-studios/frozen-sing-along-celebration/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/muppet-vision-3d/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/hollywood-studios/muppet-vision-3d/muppet-vision-3d-gallery02.jpg?1559892225794</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/630/354/90/media/disneyparksjapan-prod/disneyparksjapan_v0001/1/media/dlr/destinations/smugglers-run-interior-16x9.jpg</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/millennium-falcon-smugglers-run/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/star-wars-rise-of-the-resistance/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/media/blog/wp-content/uploads/2019/08/slrghl6n8i9o9-624x351.jpg</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/toy-story-mania/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/hollywood-studios/toy-story-mania/toy-story-mania-gallery00.jpg?1559892255928</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/destinations/hollywood-studios/toy-story-land/toy-story-slinky-dog-ride-16x9.jpg?1637954514038</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/slinky-dog-dash/</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/alien-swirling-saucers/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/disney-world/attractions/hollywood-studios/alien-swirling-saucers/toy-story-alien-swirling-saucers-entrance-16x9.jpg?1560801030851</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/twilight-zone-tower-of-terror/</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/disney/images/4/48/TowerOfTerror_MGM.jpg/revision/latest?cb=20160206020516</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/rock-and-roller-coaster-starring-aerosmith/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/gallery/attractions/hollywood-studios/rock-and-roller-coaster-starring-aerosmith/rock-and-roller-coaster-starring-aerosmith-gallery01.jpg?1551208906640</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/attractions/hollywood-studios/lightning-mcqueens-racing-academy/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/media/blog/wp-content/uploads/2019/03/mnckjvbsdkfhdsijfdsg392fs.jpg</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/entertainment/hollywood-studios/beauty-and-the-beast-live-on-stage/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/dam/wdpro-assets/parks-and-tickets/entertainment/hollywood-studios/beauty-and-the-beast-live-on-stage/beauty-and-the-beast-live-on-stage-06.jpg?1634617857407</t>
+  </si>
+  <si>
+    <t>https://disneyworld.disney.go.com/entertainment/hollywood-studios/fantasmic/</t>
+  </si>
+  <si>
+    <t>https://cdn1.parksmedia.wdprapps.disney.com/resize/mwImage/1/1600/900/75/vision-dam/digital/parks-platform/parks-global-assets/disney-world/Fantasmic16x9-16x9.jpg?2021-11-16T16:07:23+00:00</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E03DEE-4D57-1548-9F23-E107C8596AB5}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,10 +1268,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1117,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
         <v>114</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1137,10 +1308,10 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
         <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1157,10 +1328,10 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" t="s">
         <v>118</v>
-      </c>
-      <c r="F4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1177,10 +1348,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
         <v>120</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1197,10 +1368,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" t="s">
         <v>122</v>
-      </c>
-      <c r="F6" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1217,10 +1388,10 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
         <v>124</v>
-      </c>
-      <c r="F7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1237,10 +1408,10 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" t="s">
         <v>126</v>
-      </c>
-      <c r="F8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1257,10 +1428,10 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" t="s">
         <v>128</v>
-      </c>
-      <c r="F9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1277,10 +1448,10 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
         <v>130</v>
-      </c>
-      <c r="F10" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1297,10 +1468,10 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
         <v>132</v>
-      </c>
-      <c r="F11" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1317,10 +1488,10 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1337,10 +1508,10 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
         <v>136</v>
-      </c>
-      <c r="F13" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1357,10 +1528,10 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" t="s">
         <v>138</v>
-      </c>
-      <c r="F14" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1377,10 +1548,10 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1397,10 +1568,10 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" t="s">
         <v>143</v>
-      </c>
-      <c r="F16" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1417,10 +1588,10 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" t="s">
         <v>145</v>
-      </c>
-      <c r="F17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1437,10 +1608,10 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1457,10 +1628,10 @@
         <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,10 +1648,10 @@
         <v>27</v>
       </c>
       <c r="E20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" t="s">
         <v>151</v>
-      </c>
-      <c r="F20" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1497,10 +1668,10 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1517,10 +1688,10 @@
         <v>29</v>
       </c>
       <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" t="s">
         <v>182</v>
-      </c>
-      <c r="F22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1537,10 +1708,10 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" t="s">
         <v>184</v>
-      </c>
-      <c r="F23" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1557,10 +1728,10 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" t="s">
         <v>186</v>
-      </c>
-      <c r="F24" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1577,10 +1748,10 @@
         <v>32</v>
       </c>
       <c r="E25" t="s">
+        <v>187</v>
+      </c>
+      <c r="F25" t="s">
         <v>188</v>
-      </c>
-      <c r="F25" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1597,10 +1768,10 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" t="s">
         <v>190</v>
-      </c>
-      <c r="F26" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1617,10 +1788,10 @@
         <v>34</v>
       </c>
       <c r="E27" t="s">
+        <v>167</v>
+      </c>
+      <c r="F27" t="s">
         <v>168</v>
-      </c>
-      <c r="F27" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1631,16 +1802,16 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
       </c>
       <c r="E28" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" t="s">
         <v>192</v>
-      </c>
-      <c r="F28" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1651,16 +1822,16 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
         <v>36</v>
       </c>
       <c r="E29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" t="s">
         <v>194</v>
-      </c>
-      <c r="F29" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1671,16 +1842,16 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
         <v>37</v>
       </c>
       <c r="E30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30" t="s">
         <v>196</v>
-      </c>
-      <c r="F30" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1691,16 +1862,16 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
       </c>
       <c r="E31" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" t="s">
         <v>198</v>
-      </c>
-      <c r="F31" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1711,16 +1882,16 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
       </c>
       <c r="E32" t="s">
+        <v>199</v>
+      </c>
+      <c r="F32" t="s">
         <v>200</v>
-      </c>
-      <c r="F32" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,16 +1902,16 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
         <v>40</v>
       </c>
       <c r="E33" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" t="s">
         <v>202</v>
-      </c>
-      <c r="F33" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,16 +1922,16 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
         <v>41</v>
       </c>
       <c r="E34" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" t="s">
         <v>204</v>
-      </c>
-      <c r="F34" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1777,10 +1948,10 @@
         <v>55</v>
       </c>
       <c r="E35" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" t="s">
         <v>206</v>
-      </c>
-      <c r="F35" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1797,10 +1968,10 @@
         <v>44</v>
       </c>
       <c r="E36" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" t="s">
         <v>208</v>
-      </c>
-      <c r="F36" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1817,10 +1988,10 @@
         <v>45</v>
       </c>
       <c r="E37" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37" t="s">
         <v>210</v>
-      </c>
-      <c r="F37" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1837,10 +2008,10 @@
         <v>47</v>
       </c>
       <c r="E38" t="s">
+        <v>211</v>
+      </c>
+      <c r="F38" t="s">
         <v>212</v>
-      </c>
-      <c r="F38" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1857,10 +2028,10 @@
         <v>48</v>
       </c>
       <c r="E39" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" t="s">
         <v>214</v>
-      </c>
-      <c r="F39" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1877,10 +2048,10 @@
         <v>50</v>
       </c>
       <c r="E40" t="s">
+        <v>215</v>
+      </c>
+      <c r="F40" t="s">
         <v>216</v>
-      </c>
-      <c r="F40" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1897,10 +2068,10 @@
         <v>51</v>
       </c>
       <c r="E41" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" t="s">
         <v>218</v>
-      </c>
-      <c r="F41" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1917,10 +2088,10 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
+        <v>219</v>
+      </c>
+      <c r="F42" t="s">
         <v>220</v>
-      </c>
-      <c r="F42" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1937,10 +2108,10 @@
         <v>62</v>
       </c>
       <c r="E43" t="s">
+        <v>221</v>
+      </c>
+      <c r="F43" t="s">
         <v>222</v>
-      </c>
-      <c r="F43" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1957,10 +2128,10 @@
         <v>54</v>
       </c>
       <c r="E44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" t="s">
         <v>224</v>
-      </c>
-      <c r="F44" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,6 +2147,12 @@
       <c r="D45" t="s">
         <v>63</v>
       </c>
+      <c r="E45" t="s">
+        <v>225</v>
+      </c>
+      <c r="F45" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -1990,6 +2167,12 @@
       <c r="D46" t="s">
         <v>64</v>
       </c>
+      <c r="E46" t="s">
+        <v>227</v>
+      </c>
+      <c r="F46" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -2004,6 +2187,12 @@
       <c r="D47" t="s">
         <v>65</v>
       </c>
+      <c r="E47" t="s">
+        <v>229</v>
+      </c>
+      <c r="F47" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -2018,6 +2207,12 @@
       <c r="D48" t="s">
         <v>66</v>
       </c>
+      <c r="E48" t="s">
+        <v>231</v>
+      </c>
+      <c r="F48" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -2032,6 +2227,12 @@
       <c r="D49" t="s">
         <v>67</v>
       </c>
+      <c r="E49" t="s">
+        <v>233</v>
+      </c>
+      <c r="F49" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -2046,6 +2247,12 @@
       <c r="D50" t="s">
         <v>61</v>
       </c>
+      <c r="E50" t="s">
+        <v>236</v>
+      </c>
+      <c r="F50" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -2058,7 +2265,13 @@
         <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="E51" t="s">
+        <v>238</v>
+      </c>
+      <c r="F51" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2074,6 +2287,12 @@
       <c r="D52" t="s">
         <v>60</v>
       </c>
+      <c r="E52" t="s">
+        <v>239</v>
+      </c>
+      <c r="F52" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
@@ -2088,6 +2307,12 @@
       <c r="D53" t="s">
         <v>57</v>
       </c>
+      <c r="E53" t="s">
+        <v>241</v>
+      </c>
+      <c r="F53" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -2102,6 +2327,12 @@
       <c r="D54" t="s">
         <v>59</v>
       </c>
+      <c r="E54" t="s">
+        <v>244</v>
+      </c>
+      <c r="F54" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
@@ -2116,6 +2347,12 @@
       <c r="D55" t="s">
         <v>58</v>
       </c>
+      <c r="E55" t="s">
+        <v>246</v>
+      </c>
+      <c r="F55" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -2130,6 +2367,12 @@
       <c r="D56" t="s">
         <v>68</v>
       </c>
+      <c r="E56" t="s">
+        <v>248</v>
+      </c>
+      <c r="F56" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -2145,10 +2388,10 @@
         <v>71</v>
       </c>
       <c r="E57" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" t="s">
         <v>155</v>
-      </c>
-      <c r="F57" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2165,10 +2408,10 @@
         <v>72</v>
       </c>
       <c r="E58" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58" t="s">
         <v>157</v>
-      </c>
-      <c r="F58" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2185,10 +2428,10 @@
         <v>73</v>
       </c>
       <c r="E59" t="s">
+        <v>158</v>
+      </c>
+      <c r="F59" t="s">
         <v>159</v>
-      </c>
-      <c r="F59" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2205,10 +2448,10 @@
         <v>74</v>
       </c>
       <c r="E60" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" t="s">
         <v>161</v>
-      </c>
-      <c r="F60" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2225,10 +2468,10 @@
         <v>76</v>
       </c>
       <c r="E61" t="s">
+        <v>171</v>
+      </c>
+      <c r="F61" t="s">
         <v>172</v>
-      </c>
-      <c r="F61" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2245,10 +2488,10 @@
         <v>77</v>
       </c>
       <c r="E62" t="s">
+        <v>173</v>
+      </c>
+      <c r="F62" t="s">
         <v>174</v>
-      </c>
-      <c r="F62" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2265,10 +2508,10 @@
         <v>78</v>
       </c>
       <c r="E63" t="s">
+        <v>175</v>
+      </c>
+      <c r="F63" t="s">
         <v>176</v>
-      </c>
-      <c r="F63" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2285,10 +2528,10 @@
         <v>79</v>
       </c>
       <c r="E64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F64" t="s">
         <v>178</v>
-      </c>
-      <c r="F64" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2305,10 +2548,10 @@
         <v>80</v>
       </c>
       <c r="E65" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" t="s">
         <v>180</v>
-      </c>
-      <c r="F65" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2324,6 +2567,12 @@
       <c r="D66" t="s">
         <v>81</v>
       </c>
+      <c r="E66" t="s">
+        <v>250</v>
+      </c>
+      <c r="F66" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -2338,6 +2587,12 @@
       <c r="D67" t="s">
         <v>82</v>
       </c>
+      <c r="E67" t="s">
+        <v>251</v>
+      </c>
+      <c r="F67" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -2352,6 +2607,12 @@
       <c r="D68" t="s">
         <v>86</v>
       </c>
+      <c r="E68" t="s">
+        <v>253</v>
+      </c>
+      <c r="F68" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -2366,6 +2627,12 @@
       <c r="D69" t="s">
         <v>88</v>
       </c>
+      <c r="E69" t="s">
+        <v>256</v>
+      </c>
+      <c r="F69" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
@@ -2380,6 +2647,12 @@
       <c r="D70" t="s">
         <v>89</v>
       </c>
+      <c r="E70" t="s">
+        <v>257</v>
+      </c>
+      <c r="F70" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -2394,259 +2667,317 @@
       <c r="D71" t="s">
         <v>90</v>
       </c>
+      <c r="E71" t="s">
+        <v>260</v>
+      </c>
+      <c r="F71" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="E72" t="s">
+        <v>261</v>
+      </c>
+      <c r="F72" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="E73" t="s">
+        <v>264</v>
+      </c>
+      <c r="F73" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
         <v>95</v>
       </c>
+      <c r="E74" t="s">
+        <v>265</v>
+      </c>
+      <c r="F74" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D75" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="E75" t="s">
+        <v>267</v>
+      </c>
+      <c r="F75" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
         <v>98</v>
       </c>
+      <c r="E76" t="s">
+        <v>270</v>
+      </c>
+      <c r="F76" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D77" t="s">
         <v>99</v>
       </c>
+      <c r="E77" t="s">
+        <v>271</v>
+      </c>
+      <c r="F77" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>84</v>
       </c>
       <c r="C78" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D78" t="s">
-        <v>100</v>
+        <v>162</v>
+      </c>
+      <c r="E78" t="s">
+        <v>163</v>
+      </c>
+      <c r="F78" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
       </c>
       <c r="C79" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79" t="s">
         <v>101</v>
       </c>
-      <c r="D79" t="s">
-        <v>163</v>
-      </c>
       <c r="E79" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F79" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
       </c>
       <c r="C80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D80" t="s">
         <v>102</v>
       </c>
       <c r="E80" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F80" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
         <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D81" t="s">
         <v>103</v>
       </c>
       <c r="E81" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F81" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D82" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>170</v>
+        <v>273</v>
       </c>
       <c r="F82" t="s">
-        <v>171</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
         <v>84</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D83" t="s">
         <v>106</v>
       </c>
+      <c r="E83" t="s">
+        <v>275</v>
+      </c>
+      <c r="F83" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D84" t="s">
         <v>107</v>
       </c>
+      <c r="E84" t="s">
+        <v>277</v>
+      </c>
+      <c r="F84" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D85" t="s">
         <v>108</v>
       </c>
+      <c r="E85" t="s">
+        <v>279</v>
+      </c>
+      <c r="F85" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D86" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>88</v>
-      </c>
-      <c r="B87" t="s">
-        <v>84</v>
-      </c>
-      <c r="C87" t="s">
-        <v>105</v>
-      </c>
-      <c r="D87" t="s">
-        <v>110</v>
+      <c r="E86" t="s">
+        <v>281</v>
+      </c>
+      <c r="F86" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F87" xr:uid="{39E03DEE-4D57-1548-9F23-E107C8596AB5}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F87">
-      <sortCondition ref="A1:A87"/>
+  <autoFilter ref="A1:F86" xr:uid="{39E03DEE-4D57-1548-9F23-E107C8596AB5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F86">
+      <sortCondition ref="A1:A86"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>